<commit_message>
Add initial project 4 files
</commit_message>
<xml_diff>
--- a/project2_cs475/project2.xlsx
+++ b/project2_cs475/project2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryceegley/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryceegley/Desktop/cs475-Parallel-Programming/project2_cs475/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -326,11 +326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1893516672"/>
-        <c:axId val="1914842928"/>
+        <c:axId val="-447519376"/>
+        <c:axId val="-447516256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1893516672"/>
+        <c:axId val="-447519376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -447,12 +447,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1914842928"/>
+        <c:crossAx val="-447516256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1914842928"/>
+        <c:axId val="-447516256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1893516672"/>
+        <c:crossAx val="-447519376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -785,7 +785,6 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="b"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -793,11 +792,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1915718448"/>
-        <c:axId val="1913217904"/>
+        <c:axId val="-447736112"/>
+        <c:axId val="-447732992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1915718448"/>
+        <c:axId val="-447736112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,12 +912,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1913217904"/>
+        <c:crossAx val="-447732992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1913217904"/>
+        <c:axId val="-447732992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,7 +1029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1915718448"/>
+        <c:crossAx val="-447736112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1258,11 +1257,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1918064112"/>
-        <c:axId val="1918056096"/>
+        <c:axId val="-447487968"/>
+        <c:axId val="-447484848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1918064112"/>
+        <c:axId val="-447487968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,12 +1377,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1918056096"/>
+        <c:crossAx val="-447484848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1918056096"/>
+        <c:axId val="-447484848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1495,7 +1494,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1918064112"/>
+        <c:crossAx val="-447487968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1723,11 +1722,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1893239824"/>
-        <c:axId val="1914615680"/>
+        <c:axId val="-485119504"/>
+        <c:axId val="-451094144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1893239824"/>
+        <c:axId val="-485119504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1843,12 +1842,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1914615680"/>
+        <c:crossAx val="-451094144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1914615680"/>
+        <c:axId val="-451094144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1960,7 +1959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1893239824"/>
+        <c:crossAx val="-485119504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>